<commit_message>
Added home screen layout and class file. activity_main loads activity_home_screen on launch.
</commit_message>
<xml_diff>
--- a/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
@@ -58,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,7 +92,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1578,7 +1578,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Small change to burndown chart
</commit_message>
<xml_diff>
--- a/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
@@ -291,7 +291,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,7 +1578,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1607,7 @@
         <v>43384</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3">
         <v>66</v>

</xml_diff>

<commit_message>
Small update to burndown chart
</commit_message>
<xml_diff>
--- a/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
@@ -292,6 +292,18 @@
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,7 +1590,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,6 +1639,9 @@
       <c r="A3" s="1">
         <v>43385</v>
       </c>
+      <c r="B3">
+        <v>65</v>
+      </c>
       <c r="C3" s="3">
         <f>(C2-3.3)</f>
         <v>62.7</v>
@@ -1646,6 +1661,9 @@
       <c r="A4" s="1">
         <v>43386</v>
       </c>
+      <c r="B4">
+        <v>65</v>
+      </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C22" si="1">(C3-3.3)</f>
         <v>59.400000000000006</v>
@@ -1665,6 +1683,9 @@
       <c r="A5" s="1">
         <v>43387</v>
       </c>
+      <c r="B5">
+        <v>65</v>
+      </c>
       <c r="C5" s="3">
         <f t="shared" si="1"/>
         <v>56.100000000000009</v>
@@ -1683,6 +1704,9 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43388</v>
+      </c>
+      <c r="B6">
+        <v>61</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update to Burndown Chart
</commit_message>
<xml_diff>
--- a/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
@@ -304,6 +304,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,7 +1596,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +1733,9 @@
       <c r="A7" s="1">
         <v>43389</v>
       </c>
+      <c r="B7">
+        <v>61</v>
+      </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
         <v>49.500000000000014</v>
@@ -1743,6 +1752,9 @@
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43390</v>
+      </c>
+      <c r="B8">
+        <v>59</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Final Burndown chart update - completed
</commit_message>
<xml_diff>
--- a/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 1/Burndown Chart Sprint 1.xlsx
@@ -343,6 +343,15 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1629,7 +1638,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,6 +1939,9 @@
       <c r="A20" s="1">
         <v>43402</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
       <c r="C20" s="3">
         <f t="shared" si="1"/>
         <v>6.6000000000000236</v>
@@ -1939,6 +1951,9 @@
       <c r="A21" s="1">
         <v>43403</v>
       </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
       <c r="C21" s="3">
         <f t="shared" si="1"/>
         <v>3.3000000000000238</v>
@@ -1947,6 +1962,9 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43404</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="1"/>

</xml_diff>